<commit_message>
Updated code with fixes
</commit_message>
<xml_diff>
--- a/public/form_data.xlsx
+++ b/public/form_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1533,9 +1533,415 @@
         <v>General Inquiry</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>User</v>
+      </c>
+      <c r="B40" t="str">
+        <v>User</v>
+      </c>
+      <c r="C40" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D40" t="str">
+        <v>null</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="F40" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="G40" t="str">
+        <v>Interested in services</v>
+      </c>
+      <c r="H40" t="str">
+        <v>Not specified</v>
+      </c>
+      <c r="I40" t="str">
+        <v>General Inquiry</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Krissh</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Gera</v>
+      </c>
+      <c r="C41" t="str">
+        <v>gkrissh7@gmail.com</v>
+      </c>
+      <c r="D41" t="str">
+        <v>3dcarcare@gmail.com</v>
+      </c>
+      <c r="E41" t="str">
+        <v>09870305778</v>
+      </c>
+      <c r="F41" t="str">
+        <v>3d car care India</v>
+      </c>
+      <c r="G41" t="str">
+        <v>make meta ads for me</v>
+      </c>
+      <c r="H41" t="str">
+        <v>2000</v>
+      </c>
+      <c r="I41" t="str">
+        <v>Website building</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Akshan</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Aggarwal</v>
+      </c>
+      <c r="C42" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D42" t="str">
+        <v>3dcarcare@gmail.com</v>
+      </c>
+      <c r="E42" t="str">
+        <v>09870305778</v>
+      </c>
+      <c r="F42" t="str">
+        <v>3d car care India</v>
+      </c>
+      <c r="G42" t="str">
+        <v>make meta ads for me</v>
+      </c>
+      <c r="H42" t="str">
+        <v>2000</v>
+      </c>
+      <c r="I42" t="str">
+        <v>Website building</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Akshan</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Aggarwal</v>
+      </c>
+      <c r="C43" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D43" t="str">
+        <v>3dcarcare@gmail.com</v>
+      </c>
+      <c r="E43" t="str">
+        <v>09870305778</v>
+      </c>
+      <c r="F43" t="str">
+        <v>3d car care India</v>
+      </c>
+      <c r="G43" t="str">
+        <v>make meta ads for me</v>
+      </c>
+      <c r="H43" t="str">
+        <v>2000</v>
+      </c>
+      <c r="I43" t="str">
+        <v>Website building</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Krishna</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Aggarwal</v>
+      </c>
+      <c r="C44" t="str">
+        <v>aggarwalkrishna3163@gmail.com</v>
+      </c>
+      <c r="D44" t="str">
+        <v>3dcarcare@gmail.com</v>
+      </c>
+      <c r="E44" t="str">
+        <v>09870305778</v>
+      </c>
+      <c r="F44" t="str">
+        <v>3d car care India</v>
+      </c>
+      <c r="G44" t="str">
+        <v>make meta ads for me</v>
+      </c>
+      <c r="H44" t="str">
+        <v>2000</v>
+      </c>
+      <c r="I44" t="str">
+        <v>Website building</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>User</v>
+      </c>
+      <c r="B45" t="str">
+        <v>User</v>
+      </c>
+      <c r="C45" t="str">
+        <v>official.pranav02@gmail.com</v>
+      </c>
+      <c r="D45" t="str">
+        <v>null</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="F45" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="G45" t="str">
+        <v>Interested in services</v>
+      </c>
+      <c r="H45" t="str">
+        <v>Not specified</v>
+      </c>
+      <c r="I45" t="str">
+        <v>General Inquiry</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Akshan</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Aggarwal</v>
+      </c>
+      <c r="C46" t="str">
+        <v>akshanaggarwal20@gmail.com</v>
+      </c>
+      <c r="D46" t="str">
+        <v>3dcarcare@gmail.com</v>
+      </c>
+      <c r="E46" t="str">
+        <v>09870305778</v>
+      </c>
+      <c r="F46" t="str">
+        <v>3d car care India</v>
+      </c>
+      <c r="G46" t="str">
+        <v>make meta ads for me</v>
+      </c>
+      <c r="H46" t="str">
+        <v>2000</v>
+      </c>
+      <c r="I46" t="str">
+        <v>Website building</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>User</v>
+      </c>
+      <c r="B47" t="str">
+        <v>User</v>
+      </c>
+      <c r="C47" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D47" t="str">
+        <v>null</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="F47" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="G47" t="str">
+        <v>Interested in services</v>
+      </c>
+      <c r="H47" t="str">
+        <v>Not specified</v>
+      </c>
+      <c r="I47" t="str">
+        <v>General Inquiry</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>User</v>
+      </c>
+      <c r="B48" t="str">
+        <v>User</v>
+      </c>
+      <c r="C48" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D48" t="str">
+        <v>null</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="F48" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="G48" t="str">
+        <v>Interested in services</v>
+      </c>
+      <c r="H48" t="str">
+        <v>Not specified</v>
+      </c>
+      <c r="I48" t="str">
+        <v>General Inquiry</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>User</v>
+      </c>
+      <c r="B49" t="str">
+        <v>User</v>
+      </c>
+      <c r="C49" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D49" t="str">
+        <v>null</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="F49" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="G49" t="str">
+        <v>Interested in services</v>
+      </c>
+      <c r="H49" t="str">
+        <v>Not specified</v>
+      </c>
+      <c r="I49" t="str">
+        <v>General Inquiry</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Akshan</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Aggarwal</v>
+      </c>
+      <c r="C50" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D50" t="str">
+        <v>3dcarcare@gmail.com</v>
+      </c>
+      <c r="E50" t="str">
+        <v>09870305778</v>
+      </c>
+      <c r="F50" t="str">
+        <v>3d car care India</v>
+      </c>
+      <c r="G50" t="str">
+        <v>make meta ads for me</v>
+      </c>
+      <c r="H50" t="str">
+        <v>2000</v>
+      </c>
+      <c r="I50" t="str">
+        <v>Website building</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Akshan</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Aggarwal</v>
+      </c>
+      <c r="C51" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D51" t="str">
+        <v>3dcarcare@gmail.com</v>
+      </c>
+      <c r="E51" t="str">
+        <v>09870305778</v>
+      </c>
+      <c r="F51" t="str">
+        <v>3d car care India</v>
+      </c>
+      <c r="G51" t="str">
+        <v>make meta ads for me</v>
+      </c>
+      <c r="H51" t="str">
+        <v>2000</v>
+      </c>
+      <c r="I51" t="str">
+        <v>Website building</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Akshan</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Aggarwal</v>
+      </c>
+      <c r="C52" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D52" t="str">
+        <v>3D</v>
+      </c>
+      <c r="E52" t="str">
+        <v>9870305778</v>
+      </c>
+      <c r="F52" t="str">
+        <v>3D</v>
+      </c>
+      <c r="G52" t="str">
+        <v>No help</v>
+      </c>
+      <c r="H52" t="str">
+        <v>50000</v>
+      </c>
+      <c r="I52" t="str">
+        <v xml:space="preserve">Website development </v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>User</v>
+      </c>
+      <c r="B53" t="str">
+        <v>User</v>
+      </c>
+      <c r="C53" t="str">
+        <v>akshanaggarwal2005@hotmail.com</v>
+      </c>
+      <c r="D53" t="str">
+        <v>null</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="F53" t="str">
+        <v>Not provided</v>
+      </c>
+      <c r="G53" t="str">
+        <v>Interested in services</v>
+      </c>
+      <c r="H53" t="str">
+        <v>Not specified</v>
+      </c>
+      <c r="I53" t="str">
+        <v>General Inquiry</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I53"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>